<commit_message>
Update on cleaning data.
</commit_message>
<xml_diff>
--- a/data/tea wt.xlsx
+++ b/data/tea wt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/NREC_Decomp_2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216B5254-C0C5-C642-90D4-0BDA5DCA185E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11225B06-3C9F-DD49-89A3-174A2257A227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="760" windowWidth="28800" windowHeight="18000" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="14">
   <si>
     <t>tea_id</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A516A593-0A2C-7142-8637-46791FA91D9E}">
-  <dimension ref="A1:F401"/>
+  <dimension ref="A1:G433"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163:XFD163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +715,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -729,7 +732,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -746,7 +749,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -763,7 +766,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -779,8 +782,11 @@
       <c r="E20">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -797,7 +803,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -814,7 +820,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -831,7 +837,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -848,7 +854,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -865,7 +871,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -882,7 +888,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -899,7 +905,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -916,7 +922,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -933,7 +939,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -950,7 +956,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -967,7 +973,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5586,6 +5592,262 @@
         <v>400</v>
       </c>
       <c r="E401">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>501</v>
+      </c>
+      <c r="E402">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>502</v>
+      </c>
+      <c r="E403">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>503</v>
+      </c>
+      <c r="E404">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>504</v>
+      </c>
+      <c r="E405">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>505</v>
+      </c>
+      <c r="E406">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>506</v>
+      </c>
+      <c r="E407">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>507</v>
+      </c>
+      <c r="E408">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>508</v>
+      </c>
+      <c r="E409">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>509</v>
+      </c>
+      <c r="E410">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>510</v>
+      </c>
+      <c r="E411">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>511</v>
+      </c>
+      <c r="E412">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>512</v>
+      </c>
+      <c r="E413">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>513</v>
+      </c>
+      <c r="E414">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>514</v>
+      </c>
+      <c r="E415">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>515</v>
+      </c>
+      <c r="E416">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>516</v>
+      </c>
+      <c r="E417">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>517</v>
+      </c>
+      <c r="E418">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>518</v>
+      </c>
+      <c r="E419">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>519</v>
+      </c>
+      <c r="E420">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>520</v>
+      </c>
+      <c r="E421">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>521</v>
+      </c>
+      <c r="E422">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>522</v>
+      </c>
+      <c r="E423">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>523</v>
+      </c>
+      <c r="E424">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>524</v>
+      </c>
+      <c r="E425">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>525</v>
+      </c>
+      <c r="E426">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>526</v>
+      </c>
+      <c r="E427">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>527</v>
+      </c>
+      <c r="E428">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>528</v>
+      </c>
+      <c r="E429">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>529</v>
+      </c>
+      <c r="E430">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>530</v>
+      </c>
+      <c r="E431">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>551</v>
+      </c>
+      <c r="E432">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>561</v>
+      </c>
+      <c r="E433">
         <v>2.2000000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to figure out things...
still does not seem right
</commit_message>
<xml_diff>
--- a/data/tea wt.xlsx
+++ b/data/tea wt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/NREC_Decomp_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11225B06-3C9F-DD49-89A3-174A2257A227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010EC978-4023-4A4E-93B6-10F4FA863814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
+    <workbookView xWindow="1000" yWindow="760" windowWidth="28800" windowHeight="15680" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="12">
   <si>
     <t>tea_id</t>
   </si>
@@ -66,12 +66,6 @@
   </si>
   <si>
     <t>gpc</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>forgot to measure probably 2</t>
   </si>
   <si>
     <t>notes</t>
@@ -133,9 +127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +167,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -279,7 +273,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -431,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A516A593-0A2C-7142-8637-46791FA91D9E}">
   <dimension ref="A1:G433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163:XFD163"/>
+    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
+      <selection activeCell="E180" sqref="E180:G181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +451,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -783,7 +777,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3438,7 +3432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3455,7 +3449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3472,7 +3466,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3489,7 +3483,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -3502,14 +3496,8 @@
       <c r="D180">
         <v>9</v>
       </c>
-      <c r="E180" t="s">
-        <v>10</v>
-      </c>
-      <c r="F180" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -3522,14 +3510,8 @@
       <c r="D181">
         <v>10</v>
       </c>
-      <c r="E181" t="s">
-        <v>10</v>
-      </c>
-      <c r="F181" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -3546,7 +3528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -3563,7 +3545,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -3580,7 +3562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -3597,7 +3579,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -3614,7 +3596,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -3631,7 +3613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -3648,7 +3630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -3665,7 +3647,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -3682,7 +3664,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -3699,7 +3681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>

</xml_diff>

<commit_message>
Commenting on Bill's comments.
</commit_message>
<xml_diff>
--- a/data/tea wt.xlsx
+++ b/data/tea wt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/NREC_Decomp_2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17891A2A-BB21-654D-B3BC-D8A4953B3748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D72BB9-CCED-7447-B1F1-F9774B6F3D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="760" windowWidth="28800" windowHeight="15680" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{6323B2E8-4C20-D04F-8676-F62966C64EA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -167,7 +167,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -273,7 +273,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -415,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A516A593-0A2C-7142-8637-46791FA91D9E}">
   <dimension ref="A1:G433"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A256" sqref="A256"/>
+    <sheetView tabSelected="1" topLeftCell="A419" workbookViewId="0">
+      <selection activeCell="E182" sqref="E182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3496,6 +3496,9 @@
       <c r="D180">
         <v>9</v>
       </c>
+      <c r="E180">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181">
@@ -3509,6 +3512,9 @@
       </c>
       <c r="D181">
         <v>10</v>
+      </c>
+      <c r="E181">
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>